<commit_message>
chore(data): update mas data
</commit_message>
<xml_diff>
--- a/data/S$NEER.xlsx
+++ b/data/S$NEER.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" saveExternalLinkValues="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6BAE58-A813-4FCD-80FD-911BE2E9ADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC13DD-B39F-4D67-802C-D195372C9F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="9">'2017-18'!$A$1:$B$112</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'2019-20'!$A$1:$B$113</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'2021-22'!$A$1:$C$115</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="12">'2023-24'!$A$1:$C$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="12">'2023-24'!$A$1:$C$89</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'1999-00'!$1:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2001-02'!$1:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2003-04'!$1:$7</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="122">
   <si>
     <t xml:space="preserve">1999 Jan 8  </t>
   </si>
@@ -425,7 +425,7 @@
     <t xml:space="preserve">2024 Jan 5  </t>
   </si>
   <si>
-    <t>Data Last Updated: 3 June 2024, 12pm</t>
+    <t>Data Last Updated: 1 July 2024, 12pm</t>
   </si>
 </sst>
 </file>
@@ -5656,13 +5656,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q118" sqref="Q118"/>
+      <selection pane="bottomRight" activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6513,33 +6513,77 @@
       <c r="G81" s="16"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
+      <c r="A82" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="11">
+        <v>139.09</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="15"/>
       <c r="G82" s="16"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="19">
+        <v>14</v>
+      </c>
+      <c r="B83" s="11">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="D83" s="23"/>
+      <c r="E83" s="15"/>
       <c r="G83" s="16"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
-        <v>121</v>
-      </c>
+      <c r="A84" s="19">
+        <v>21</v>
+      </c>
+      <c r="B84" s="11">
+        <v>139.19</v>
+      </c>
+      <c r="D84" s="23"/>
+      <c r="E84" s="15"/>
       <c r="G84" s="16"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="19">
+        <v>28</v>
+      </c>
+      <c r="B85" s="11">
+        <v>139.18</v>
+      </c>
+      <c r="D85" s="23"/>
+      <c r="E85" s="15"/>
       <c r="G85" s="16"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
       <c r="G86" s="16"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G87" s="16"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="G88" s="16"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="24"/>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="16"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G90" s="16"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G91" s="16"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="16"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -15543,62 +15587,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">bcf8a310-0c7f-418e-8782-91dee3898d42</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Url>https://home.dms.mas.gov.sg/_layouts/15/MASGlobalID/DocAveRedirect.aspx?DocId=bcf8a310-0c7f-418e-8782-91dee3898d42&amp;SiteID=5a6bb544-3bf9-4cf9-9775-b4c0c62fec92_eb98edff-86eb-4b42-ad62-1a553ba43033</Url>
-      <Description>bcf8a310-0c7f-418e-8782-91dee3898d42</Description>
-    </_dlc_DocIdUrl>
-    <Workflow xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Workflow>
-    <b1f4bea4dbaa4479a68e8cee40e226b9 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b1f4bea4dbaa4479a68e8cee40e226b9>
-    <pb016fef86a642189c1d23bc7cb88f0e xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </pb016fef86a642189c1d23bc7cb88f0e>
-    <h63e849b28044e64bfbe5f5fa7b8c866 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h63e849b28044e64bfbe5f5fa7b8c866>
-    <TaxCatchAll xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b"/>
-    <a2b7da5d9b994f938881636f0a7c63d6 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </a2b7da5d9b994f938881636f0a7c63d6>
-    <g5d17599f0654139ac247b509bd42854 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g5d17599f0654139ac247b509bd42854>
-    <h6ac82fb60e7404bb7825d9f5fed2f8a xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6ac82fb60e7404bb7825d9f5fed2f8a>
-    <ee94ffbfe3174827a439912fa17811b9 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ee94ffbfe3174827a439912fa17811b9>
-    <c569feee562949f193efcc6c33983d2e xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c569feee562949f193efcc6c33983d2e>
-    <Document_x0020_Date xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">2021-10-28T00:15:01+00:00</Document_x0020_Date>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="afabadb4-2257-48ec-869f-64421b8f49cd" ContentTypeId="0x0101003618E443DE96424ABE734F4442FBF2B301" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="MAS Team Document" ma:contentTypeID="0x0101003618E443DE96424ABE734F4442FBF2B30100A049349C955CBC409819E2464551F052" ma:contentTypeVersion="57" ma:contentTypeDescription="Create a new document specific to MAS Team Collaboration." ma:contentTypeScope="" ma:versionID="99b6c2e5e6a62f4a47c2c9b80d9ed879">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a90f38b-cee7-4289-b705-21e4ceceb96b" xmlns:ns4="eb98edff-86eb-4b42-ad62-1a553ba43033" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1700ab521322483cad2fe357906d8f66" ns2:_="" ns4:_="">
     <xsd:import namespace="3a90f38b-cee7-4289-b705-21e4ceceb96b"/>
@@ -15875,25 +15868,58 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ABF87FA-AF0C-4CFA-A2B7-3FDB3EF177BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3a90f38b-cee7-4289-b705-21e4ceceb96b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">bcf8a310-0c7f-418e-8782-91dee3898d42</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Url>https://home.dms.mas.gov.sg/_layouts/15/MASGlobalID/DocAveRedirect.aspx?DocId=bcf8a310-0c7f-418e-8782-91dee3898d42&amp;SiteID=5a6bb544-3bf9-4cf9-9775-b4c0c62fec92_eb98edff-86eb-4b42-ad62-1a553ba43033</Url>
+      <Description>bcf8a310-0c7f-418e-8782-91dee3898d42</Description>
+    </_dlc_DocIdUrl>
+    <Workflow xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Workflow>
+    <b1f4bea4dbaa4479a68e8cee40e226b9 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b1f4bea4dbaa4479a68e8cee40e226b9>
+    <pb016fef86a642189c1d23bc7cb88f0e xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </pb016fef86a642189c1d23bc7cb88f0e>
+    <h63e849b28044e64bfbe5f5fa7b8c866 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h63e849b28044e64bfbe5f5fa7b8c866>
+    <TaxCatchAll xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b"/>
+    <a2b7da5d9b994f938881636f0a7c63d6 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </a2b7da5d9b994f938881636f0a7c63d6>
+    <g5d17599f0654139ac247b509bd42854 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g5d17599f0654139ac247b509bd42854>
+    <h6ac82fb60e7404bb7825d9f5fed2f8a xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6ac82fb60e7404bb7825d9f5fed2f8a>
+    <ee94ffbfe3174827a439912fa17811b9 xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ee94ffbfe3174827a439912fa17811b9>
+    <c569feee562949f193efcc6c33983d2e xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c569feee562949f193efcc6c33983d2e>
+    <Document_x0020_Date xmlns="3a90f38b-cee7-4289-b705-21e4ceceb96b">2021-10-28T00:15:01+00:00</Document_x0020_Date>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98C795BD-E3DF-4E21-A86C-BA6DB881499A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF67AFA4-B68A-4B26-819B-29BF0526CEAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -15901,7 +15927,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A6E1E2-BE9F-46D5-A72A-8F4CBCC2457C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15918,4 +15944,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ABF87FA-AF0C-4CFA-A2B7-3FDB3EF177BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3a90f38b-cee7-4289-b705-21e4ceceb96b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98C795BD-E3DF-4E21-A86C-BA6DB881499A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>